<commit_message>
Generate new diagrams for seminar presentation
</commit_message>
<xml_diff>
--- a/data/processed/powercalcs.xlsx
+++ b/data/processed/powercalcs.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="63">
   <si>
     <t>Mote</t>
   </si>
@@ -162,10 +162,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Life</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Sleep</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -206,10 +202,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>(days)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Low-Power A</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -228,31 +220,31 @@
     <t>(v)</t>
   </si>
   <si>
-    <t>Avg</t>
-  </si>
-  <si>
-    <t>(mW)</t>
-  </si>
-  <si>
     <t>50 wH</t>
   </si>
   <si>
-    <t>Sleep</t>
-  </si>
-  <si>
-    <t>LowPwr A</t>
-  </si>
-  <si>
-    <t>LowPwr B</t>
-  </si>
-  <si>
-    <t>ThermoS.</t>
-  </si>
-  <si>
-    <t>Existing</t>
-  </si>
-  <si>
     <t>Model</t>
+  </si>
+  <si>
+    <t>mW</t>
+  </si>
+  <si>
+    <t>days</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>Sleeping</t>
+  </si>
+  <si>
+    <t>ThermoSense</t>
+  </si>
+  <si>
+    <t>Low Pwr A</t>
+  </si>
+  <si>
+    <t>Low Pwr B</t>
   </si>
 </sst>
 </file>
@@ -357,6 +349,1975 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$41:$J$42</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>days</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$43:$A$47</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Current</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sleeping</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ThermoSense</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Low Pwr A</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Low Pwr B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$43:$J$47</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>8.1431102772566195</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.323682608188131</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>130.97782807326374</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>438.07725439812049</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4718.1580009202289</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-839924976"/>
+        <c:axId val="-839930960"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-839924976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="t" anchorCtr="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-839930960"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-839930960"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Life</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" baseline="0"/>
+                  <a:t> (days)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-AU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-839924976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$41:$I$42</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>mW</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.0" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$43:$A$47</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Current</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sleeping</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ThermoSense</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Low Pwr A</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Low Pwr B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$43:$I$47</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>255.84</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>169.05119999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.906000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.7556299999999991</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.44155650000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-833817392"/>
+        <c:axId val="-833815216"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-833817392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Prototype</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" baseline="0"/>
+                  <a:t> Version</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-AU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="t" anchorCtr="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-833815216"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-833815216"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Power Consumption (mW)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-833817392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>274674</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>66748</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>570023</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>41349</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>265814</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>70885</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>561163</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>45485</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -625,7 +2586,7 @@
   <dimension ref="A2:M66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScale="129" zoomScaleNormal="129" zoomScalePageLayoutView="129" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -798,7 +2759,7 @@
         <v>11</v>
       </c>
       <c r="K13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1250,68 +3211,62 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41" t="s">
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D41" t="s">
         <v>38</v>
       </c>
       <c r="E41" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F41" t="s">
         <v>38</v>
       </c>
       <c r="G41" t="s">
+        <v>40</v>
+      </c>
+      <c r="H41" t="s">
         <v>41</v>
-      </c>
-      <c r="H41" t="s">
-        <v>42</v>
       </c>
       <c r="I41" t="s">
         <v>56</v>
       </c>
       <c r="J41" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C42" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" t="s">
         <v>46</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
+        <v>53</v>
+      </c>
+      <c r="F42" t="s">
         <v>47</v>
       </c>
-      <c r="E42" t="s">
-        <v>55</v>
-      </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>48</v>
       </c>
-      <c r="G42" t="s">
-        <v>49</v>
-      </c>
       <c r="H42" t="s">
-        <v>49</v>
-      </c>
-      <c r="I42" t="s">
-        <v>57</v>
-      </c>
-      <c r="J42" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B43" t="s">
         <v>35</v>
@@ -1326,7 +3281,7 @@
         <v>4.92</v>
       </c>
       <c r="F43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G43" s="9">
         <f>1/5</f>
@@ -1380,22 +3335,22 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B45" t="s">
         <v>34</v>
       </c>
       <c r="C45" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D45" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E45">
         <v>3.3</v>
       </c>
       <c r="F45" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G45" s="6">
         <f>1/5</f>
@@ -1413,7 +3368,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B46" t="s">
         <v>37</v>
@@ -1449,7 +3404,7 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B47" t="s">
         <v>37</v>
@@ -1491,7 +3446,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B49" t="s">
         <v>36</v>
@@ -1625,7 +3580,7 @@
         <v>50000</v>
       </c>
       <c r="K56" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
@@ -1740,5 +3695,6 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>